<commit_message>
SCD0172 - Melakukan Proses Pemantauan pada Menu Pipeline
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0172_Melakukan Proses Pemantauan pada Menu Pipeline.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0172_Melakukan Proses Pemantauan pada Menu Pipeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9743E2-B2F3-4E70-803E-7FE303342418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2866090E-1DDD-4AAC-A0DB-8780DF4F10ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>SIDEBAR_SUBMENU_SUBMENU</t>
   </si>
@@ -178,7 +178,7 @@
     <t>BNIMF - computer</t>
   </si>
   <si>
-    <t>UFT Test Add Leads Prospek BNIMF 05</t>
+    <t>UFT Test Add Leads Prospek BNIMF 08</t>
   </si>
 </sst>
 </file>
@@ -598,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -797,12 +797,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="B3" s="4"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6"/>
       <c r="I3" s="3"/>

</xml_diff>

<commit_message>
SCD0172--Update Digisales_Filezilla.qfl and create download file on server digisales
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0172_Melakukan Proses Pemantauan pada Menu Pipeline.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0172_Melakukan Proses Pemantauan pada Menu Pipeline.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2866090E-1DDD-4AAC-A0DB-8780DF4F10ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1642F46-1C16-4C51-BBED-336CACB8666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SCD0176" sheetId="2" r:id="rId1"/>
+    <sheet name="SCD0172" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>SIDEBAR_SUBMENU_SUBMENU</t>
   </si>
@@ -103,82 +103,78 @@
     <t>Jl. Pasar Minggu</t>
   </si>
   <si>
-    <t>DGS-191</t>
-  </si>
-  <si>
-    <t>Validasi pada tahapan Follow Up menggunakan User Sales yang Kode Outletnya masuk ke dalam mappingan Cabang BNI Multifinance (Kolom Cabang BNI Multifinance tidak kosong pada Parameter Mapping Kode Outlet BNI dengan BNI Multifinance )</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> · Login pada aplikasi Digi Sales dengan menggunakan user Sales 
- · Masuk ke Menu Pipeline tab Follow Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Terdapat  penambahan drop down di field Nama Produk untuk mengakomodir produk BNI Multifinance, yaitu sebagai berikut:
- a. BNIMF - Kendaraan Roda 4 (Baru / Bekas)
- b. BNIMF - Kendaraan Roda 2 (Baru)
- c. BNIMF - Elektronik
- d. BNIMF - Peralatan Rumah Tangga
- e. BNIMF - Jasa Pendidikan
- f. BNIMF - Jasa Pernikahan
- g. BNIMF - KPR / KPA (Baru / Bekas)
- h. BNIMF - Renovasi Rumah
- i. BNIMF - Car Ownership Program (COP)
- j. BNIMF - Motorcycle Ownership Program (MOP)
- k. BNIMF - Computer / Laptop Ownership Program (COOP)</t>
-  </si>
-  <si>
     <t>TEXT8</t>
   </si>
   <si>
-    <t>QUERY1</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY1</t>
-  </si>
-  <si>
-    <t>Check npp sales memiliki kode outlet untuk bni multifinance</t>
-  </si>
-  <si>
     <t>Tertarik</t>
   </si>
   <si>
-    <t>USER_DB</t>
-  </si>
-  <si>
-    <t>PASSWORD_DB</t>
-  </si>
-  <si>
     <t>HOSTNAME</t>
   </si>
   <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>4eFfEJAA!</t>
-  </si>
-  <si>
-    <t>192.168.232.6</t>
-  </si>
-  <si>
-    <t>QUERY2</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY2</t>
-  </si>
-  <si>
-    <t>QUERY3</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY3</t>
-  </si>
-  <si>
     <t>TEXT9</t>
   </si>
   <si>
     <t>BNIMF - computer</t>
   </si>
   <si>
-    <t>UFT Test Add Leads Prospek BNIMF 08</t>
+    <t>DGS-187</t>
+  </si>
+  <si>
+    <t>Melakukan Proses Pemantauan pada Menu Pipeline</t>
+  </si>
+  <si>
+    <t>1. login digisales mobile
+2. add prospek di menu store prospek
+3. leads prospek tersebut di add to cart
+4. setelah masuk ke pipeline - cart
+5. add ke pipeline  - follow up
+6. klik icon dibawah kemudian icon tanda panah kanan
+7. masuk ke lanjut follow up isi semua field dan pilih produk BNIMF
+8. masuk di pipeline monitoring
+9. file excel terexport, download dari server digisales
+10. kirim file ke path /bnimf_daily -&gt; di tc 9
+11. berikan approved atau rejected pada status file excel
+12 kirim file ke path / ftp_done_proces -&gt; tc 12
+13. file sampai di pipeline closing atau tidak closing sesuai status yg diberikan approved atau rejected</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Berhasil 
+ - Akan melalui proses tahapan existing, yaitu sbg berikut: 
+ Cart Followup Monitoring  Clossing / Tidak Closing</t>
+  </si>
+  <si>
+    <t>1. Login ke server digisales menggunakan tool filezilla
+2. Buka storage server
+3. Masuk ke remote site "/BNIMultifinance/in/archive"
+4. Download File BNIMF</t>
+  </si>
+  <si>
+    <t>Download File BNIMF dari Server</t>
+  </si>
+  <si>
+    <t>Berhasil Download File BNIMF</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>guest</t>
+  </si>
+  <si>
+    <t>digisales123</t>
+  </si>
+  <si>
+    <t>192.168.231.13</t>
+  </si>
+  <si>
+    <t>/BNIMultifinance/in/archive</t>
+  </si>
+  <si>
+    <t>BNIMF_sent_04042022_104324.xlsx</t>
+  </si>
+  <si>
+    <t>UFT Test Leads Prospek 02</t>
   </si>
 </sst>
 </file>
@@ -244,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -265,30 +261,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAF5E5-8229-45B3-AC11-8AED029F52F4}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,12 +627,13 @@
     <col min="18" max="18" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.42578125" customWidth="1"/>
-    <col min="21" max="21" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.85546875" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="15.42578125" customWidth="1"/>
-    <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -687,122 +692,121 @@
         <v>24</v>
       </c>
       <c r="S1" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" t="s">
+        <v>30</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" s="10" customFormat="1" ht="191.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="18">
+        <v>22914</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>12970</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
+      <c r="U2" s="14"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+    </row>
+    <row r="3" spans="1:29" ht="51" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
-        <v>42</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="C3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="L3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="X1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="11">
-        <v>22914</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="12">
-        <v>12970</v>
-      </c>
-      <c r="R2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="17"/>
-      <c r="Y2" s="17"/>
-      <c r="Z2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="6"/>
-      <c r="I3" s="3"/>
       <c r="O3" s="1"/>
       <c r="P3" s="2"/>
+      <c r="U3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>

</xml_diff>

<commit_message>
Added Function To Open lasted Download File
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0172_Melakukan Proses Pemantauan pada Menu Pipeline.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0172_Melakukan Proses Pemantauan pada Menu Pipeline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1642F46-1C16-4C51-BBED-336CACB8666E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC3950D-A8C3-4D49-AD03-0C3CD77B521C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,7 +174,7 @@
     <t>BNIMF_sent_04042022_104324.xlsx</t>
   </si>
   <si>
-    <t>UFT Test Leads Prospek 02</t>
+    <t>UFT Test Leads Prospek 04</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>